<commit_message>
Kontrola zemi vysledna tabulka
</commit_message>
<xml_diff>
--- a/Projekt_pomocne_tabulky.xlsx
+++ b/Projekt_pomocne_tabulky.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3642" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3835" uniqueCount="683">
   <si>
     <t>economies</t>
   </si>
@@ -2047,9 +2047,6 @@
     <t>4cm</t>
   </si>
   <si>
-    <t>Caribbean Netherlands</t>
-  </si>
-  <si>
     <t>Faeroe Islands</t>
   </si>
   <si>
@@ -2078,6 +2075,9 @@
   </si>
   <si>
     <t>religions</t>
+  </si>
+  <si>
+    <t>výsledná tabulka</t>
   </si>
 </sst>
 </file>
@@ -2461,10 +2461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G263"/>
+  <dimension ref="A1:I263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="G106" sqref="G106"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2472,9 +2472,10 @@
     <col min="1" max="1" width="11.21875" customWidth="1"/>
     <col min="2" max="6" width="20.33203125" customWidth="1"/>
     <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" s="12" t="s">
         <v>281</v>
       </c>
@@ -2482,7 +2483,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>282</v>
       </c>
@@ -2495,7 +2496,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>288</v>
       </c>
@@ -2515,10 +2516,13 @@
         <v>283</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -2534,8 +2538,11 @@
       <c r="G4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -2551,8 +2558,11 @@
       <c r="G5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -2568,8 +2578,11 @@
       <c r="G6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -2580,7 +2593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -2596,8 +2609,11 @@
       <c r="G8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -2613,8 +2629,11 @@
       <c r="G9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>219</v>
       </c>
@@ -2622,7 +2641,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>220</v>
       </c>
@@ -2630,7 +2649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -2646,8 +2665,11 @@
       <c r="G12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -2663,8 +2685,11 @@
       <c r="G13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -2680,19 +2705,19 @@
       <c r="G14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="G15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>11</v>
       </c>
@@ -2707,10 +2732,13 @@
         <v>11</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>12</v>
       </c>
@@ -2727,10 +2755,13 @@
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="I17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -2744,10 +2775,13 @@
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="I18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>14</v>
       </c>
@@ -2761,10 +2795,13 @@
         <v>221</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+      <c r="I19" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -2781,10 +2818,13 @@
         <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="I20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>16</v>
       </c>
@@ -2801,10 +2841,13 @@
         <v>16</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="I21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -2818,10 +2861,13 @@
         <v>17</v>
       </c>
       <c r="G22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="I22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>18</v>
       </c>
@@ -2838,10 +2884,13 @@
         <v>18</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="I23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>19</v>
       </c>
@@ -2858,10 +2907,13 @@
         <v>19</v>
       </c>
       <c r="G24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="I24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>20</v>
       </c>
@@ -2875,10 +2927,13 @@
         <v>20</v>
       </c>
       <c r="G25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="I25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>21</v>
       </c>
@@ -2892,10 +2947,13 @@
         <v>21</v>
       </c>
       <c r="G26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="I26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>22</v>
       </c>
@@ -2903,10 +2961,10 @@
         <v>22</v>
       </c>
       <c r="G27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>23</v>
       </c>
@@ -2920,10 +2978,13 @@
         <v>23</v>
       </c>
       <c r="G28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="I28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>24</v>
       </c>
@@ -2940,10 +3001,13 @@
         <v>24</v>
       </c>
       <c r="G29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="I29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>25</v>
       </c>
@@ -2957,10 +3021,13 @@
         <v>25</v>
       </c>
       <c r="G30" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="I30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>26</v>
       </c>
@@ -2974,18 +3041,21 @@
         <v>26</v>
       </c>
       <c r="G31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="I31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
         <v>222</v>
       </c>
       <c r="G32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>27</v>
       </c>
@@ -3002,26 +3072,29 @@
         <v>27</v>
       </c>
       <c r="G33" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="I33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>28</v>
       </c>
       <c r="G34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
         <v>223</v>
       </c>
       <c r="G35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
         <v>29</v>
       </c>
@@ -3035,10 +3108,13 @@
         <v>224</v>
       </c>
       <c r="G36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I36" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>30</v>
       </c>
@@ -3055,10 +3131,13 @@
         <v>30</v>
       </c>
       <c r="G37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="I37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>31</v>
       </c>
@@ -3072,10 +3151,13 @@
         <v>31</v>
       </c>
       <c r="G38" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="I38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
         <v>265</v>
       </c>
@@ -3083,10 +3165,13 @@
         <v>265</v>
       </c>
       <c r="G39" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="I39" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>32</v>
       </c>
@@ -3099,11 +3184,11 @@
       <c r="E40" t="s">
         <v>32</v>
       </c>
-      <c r="G40" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>33</v>
       </c>
@@ -3113,11 +3198,11 @@
       <c r="E41" t="s">
         <v>33</v>
       </c>
-      <c r="G41" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>34</v>
       </c>
@@ -3130,11 +3215,11 @@
       <c r="E42" t="s">
         <v>34</v>
       </c>
-      <c r="G42" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>35</v>
       </c>
@@ -3147,11 +3232,11 @@
       <c r="E43" t="s">
         <v>35</v>
       </c>
-      <c r="G43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>36</v>
       </c>
@@ -3166,18 +3251,21 @@
         <v>36</v>
       </c>
       <c r="G44" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="I44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
         <v>225</v>
       </c>
       <c r="G45" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>37</v>
       </c>
@@ -3185,10 +3273,10 @@
         <v>37</v>
       </c>
       <c r="G46" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>38</v>
       </c>
@@ -3202,10 +3290,13 @@
         <v>38</v>
       </c>
       <c r="G47" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="I47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>39</v>
       </c>
@@ -3219,18 +3310,21 @@
         <v>39</v>
       </c>
       <c r="G48" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="I48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>40</v>
       </c>
       <c r="G49" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>41</v>
       </c>
@@ -3247,14 +3341,20 @@
         <v>41</v>
       </c>
       <c r="G50" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="I50" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>42</v>
       </c>
       <c r="C51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" t="s">
         <v>42</v>
       </c>
       <c r="E51" s="4"/>
@@ -3262,26 +3362,26 @@
         <v>42</v>
       </c>
       <c r="G51" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="I51" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
         <v>226</v>
       </c>
-      <c r="G52" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
         <v>227</v>
       </c>
       <c r="G53" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>43</v>
       </c>
@@ -3298,10 +3398,13 @@
         <v>43</v>
       </c>
       <c r="G54" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="I54" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>44</v>
       </c>
@@ -3315,10 +3418,13 @@
         <v>44</v>
       </c>
       <c r="G55" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="I55" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>45</v>
       </c>
@@ -3326,10 +3432,10 @@
         <v>284</v>
       </c>
       <c r="G56" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57" s="2" t="s">
         <v>46</v>
       </c>
@@ -3342,8 +3448,11 @@
       <c r="E57" s="2" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I57" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
         <v>228</v>
       </c>
@@ -3353,8 +3462,11 @@
       <c r="E58" s="2" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>47</v>
       </c>
@@ -3370,8 +3482,14 @@
       <c r="F59" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G59" t="s">
+        <v>47</v>
+      </c>
+      <c r="I59" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B60" s="2" t="s">
         <v>48</v>
       </c>
@@ -3390,8 +3508,11 @@
       <c r="G60" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I60" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>49</v>
       </c>
@@ -3407,8 +3528,14 @@
       <c r="F61" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G61" t="s">
+        <v>49</v>
+      </c>
+      <c r="I61" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>50</v>
       </c>
@@ -3424,13 +3551,22 @@
       <c r="F62" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G62" t="s">
+        <v>50</v>
+      </c>
+      <c r="I62" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G63" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>52</v>
       </c>
@@ -3446,8 +3582,14 @@
       <c r="F64" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G64" t="s">
+        <v>52</v>
+      </c>
+      <c r="I64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
         <v>53</v>
       </c>
@@ -3466,8 +3608,11 @@
       <c r="G65" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I65" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>54</v>
       </c>
@@ -3486,8 +3631,11 @@
       <c r="G66" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
         <v>270</v>
       </c>
@@ -3497,8 +3645,11 @@
       <c r="G67" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I67" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>55</v>
       </c>
@@ -3514,8 +3665,11 @@
       <c r="G68" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I68" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>56</v>
       </c>
@@ -3531,8 +3685,11 @@
       <c r="G69" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I69" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>57</v>
       </c>
@@ -3551,8 +3708,11 @@
       <c r="G70" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I70" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
         <v>229</v>
       </c>
@@ -3560,7 +3720,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>58</v>
       </c>
@@ -3579,8 +3739,11 @@
       <c r="G72" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I72" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>59</v>
       </c>
@@ -3596,8 +3759,11 @@
       <c r="G73" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I73" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>60</v>
       </c>
@@ -3616,8 +3782,11 @@
       <c r="G74" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I74" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>61</v>
       </c>
@@ -3633,8 +3802,11 @@
       <c r="G75" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I75" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>62</v>
       </c>
@@ -3650,8 +3822,11 @@
       <c r="G76" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I76" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>63</v>
       </c>
@@ -3668,10 +3843,13 @@
         <v>63</v>
       </c>
       <c r="G77" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
+        <v>672</v>
+      </c>
+      <c r="I77" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B78" s="2" t="s">
         <v>64</v>
       </c>
@@ -3687,8 +3865,11 @@
       <c r="G78" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I78" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>65</v>
       </c>
@@ -3704,16 +3885,19 @@
       <c r="F79" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I79" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C80" t="s">
         <v>230</v>
       </c>
       <c r="G80" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>66</v>
       </c>
@@ -3721,10 +3905,10 @@
         <v>66</v>
       </c>
       <c r="G81" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>67</v>
       </c>
@@ -3743,8 +3927,11 @@
       <c r="G82" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I82" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>68</v>
       </c>
@@ -3763,8 +3950,11 @@
       <c r="G83" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I83" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>69</v>
       </c>
@@ -3783,8 +3973,11 @@
       <c r="G84" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I84" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C85" t="s">
         <v>232</v>
       </c>
@@ -3792,7 +3985,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>70</v>
       </c>
@@ -3803,7 +3996,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C87" t="s">
         <v>233</v>
       </c>
@@ -3811,7 +4004,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>71</v>
       </c>
@@ -3827,8 +4020,11 @@
       <c r="G88" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I88" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>72</v>
       </c>
@@ -3844,8 +4040,11 @@
       <c r="G89" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I89" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>73</v>
       </c>
@@ -3861,8 +4060,11 @@
       <c r="G90" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I90" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>74</v>
       </c>
@@ -3881,8 +4083,11 @@
       <c r="G91" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I91" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>75</v>
       </c>
@@ -3901,8 +4106,11 @@
       <c r="G92" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I92" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>76</v>
       </c>
@@ -3913,7 +4121,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>77</v>
       </c>
@@ -3932,8 +4140,11 @@
       <c r="G94" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I94" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>78</v>
       </c>
@@ -3944,7 +4155,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>79</v>
       </c>
@@ -3960,8 +4171,11 @@
       <c r="G96" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I96" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>80</v>
       </c>
@@ -3972,7 +4186,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>81</v>
       </c>
@@ -3983,7 +4197,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C99" t="s">
         <v>81</v>
       </c>
@@ -3999,8 +4213,11 @@
       <c r="G99" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I99" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C100" t="s">
         <v>235</v>
       </c>
@@ -4008,7 +4225,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>82</v>
       </c>
@@ -4024,8 +4241,11 @@
       <c r="G101" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I101" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>83</v>
       </c>
@@ -4041,8 +4261,11 @@
       <c r="G102" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I102" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>84</v>
       </c>
@@ -4058,8 +4281,11 @@
       <c r="G103" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I103" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>85</v>
       </c>
@@ -4075,8 +4301,11 @@
       <c r="G104" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I104" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C105" t="s">
         <v>236</v>
       </c>
@@ -4084,7 +4313,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C106" s="2" t="s">
         <v>237</v>
       </c>
@@ -4095,10 +4324,13 @@
         <v>272</v>
       </c>
       <c r="G106" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
+        <v>680</v>
+      </c>
+      <c r="I106" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>86</v>
       </c>
@@ -4114,8 +4346,11 @@
       <c r="G107" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I107" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
         <v>87</v>
       </c>
@@ -4129,7 +4364,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
         <v>88</v>
       </c>
@@ -4148,8 +4383,11 @@
       <c r="G109" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I109" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
         <v>89</v>
       </c>
@@ -4168,8 +4406,11 @@
       <c r="G110" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I110" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
         <v>90</v>
       </c>
@@ -4188,8 +4429,11 @@
       <c r="G111" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I111" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>91</v>
       </c>
@@ -4208,8 +4452,11 @@
       <c r="G112" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I112" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
         <v>92</v>
       </c>
@@ -4228,8 +4475,11 @@
       <c r="G113" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I113" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
         <v>93</v>
       </c>
@@ -4248,8 +4498,11 @@
       <c r="G114" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I114" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>94</v>
       </c>
@@ -4268,8 +4521,11 @@
       <c r="G115" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I115" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
         <v>95</v>
       </c>
@@ -4280,7 +4536,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>96</v>
       </c>
@@ -4299,8 +4555,11 @@
       <c r="G117" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I117" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
         <v>97</v>
       </c>
@@ -4319,8 +4578,11 @@
       <c r="G118" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I118" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
         <v>98</v>
       </c>
@@ -4339,8 +4601,11 @@
       <c r="G119" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I119" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>99</v>
       </c>
@@ -4359,8 +4624,11 @@
       <c r="G120" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I120" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C121" t="s">
         <v>238</v>
       </c>
@@ -4368,7 +4636,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B122" t="s">
         <v>100</v>
       </c>
@@ -4387,8 +4655,11 @@
       <c r="G122" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I122" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B123" t="s">
         <v>101</v>
       </c>
@@ -4407,8 +4678,11 @@
       <c r="G123" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I123" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="124" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
         <v>102</v>
       </c>
@@ -4427,8 +4701,11 @@
       <c r="G124" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I124" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="125" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B125" t="s">
         <v>103</v>
       </c>
@@ -4439,7 +4716,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
         <v>104</v>
       </c>
@@ -4447,7 +4724,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B127" s="2" t="s">
         <v>105</v>
       </c>
@@ -4466,8 +4743,11 @@
       <c r="G127" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I127" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="128" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B128" t="s">
         <v>106</v>
       </c>
@@ -4480,8 +4760,11 @@
       <c r="G128" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I128" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="129" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B129" t="s">
         <v>107</v>
       </c>
@@ -4500,8 +4783,11 @@
       <c r="G129" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I129" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="130" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B130" t="s">
         <v>108</v>
       </c>
@@ -4517,8 +4803,11 @@
       <c r="G130" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I130" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="131" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B131" t="s">
         <v>109</v>
       </c>
@@ -4534,8 +4823,11 @@
       <c r="G131" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I131" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="132" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B132" t="s">
         <v>110</v>
       </c>
@@ -4554,8 +4846,11 @@
       <c r="G132" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I132" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="133" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B133" t="s">
         <v>111</v>
       </c>
@@ -4571,8 +4866,11 @@
       <c r="G133" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I133" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="134" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B134" t="s">
         <v>112</v>
       </c>
@@ -4586,10 +4884,13 @@
         <v>112</v>
       </c>
       <c r="G134" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.3">
+        <v>675</v>
+      </c>
+      <c r="I134" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="135" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B135" t="s">
         <v>113</v>
       </c>
@@ -4605,8 +4906,11 @@
       <c r="G135" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I135" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="136" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B136" s="2" t="s">
         <v>114</v>
       </c>
@@ -4625,8 +4929,11 @@
       <c r="G136" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I136" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="137" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B137" t="s">
         <v>115</v>
       </c>
@@ -4642,8 +4949,11 @@
       <c r="G137" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I137" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="138" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B138" t="s">
         <v>116</v>
       </c>
@@ -4662,8 +4972,11 @@
       <c r="G138" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I138" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="139" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B139" t="s">
         <v>117</v>
       </c>
@@ -4682,8 +4995,11 @@
       <c r="G139" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I139" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="140" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B140" s="2" t="s">
         <v>118</v>
       </c>
@@ -4699,8 +5015,11 @@
       <c r="G140" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I140" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="141" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F141" t="s">
         <v>285</v>
       </c>
@@ -4708,7 +5027,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B142" t="s">
         <v>119</v>
       </c>
@@ -4727,8 +5046,11 @@
       <c r="G142" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I142" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="143" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B143" t="s">
         <v>120</v>
       </c>
@@ -4747,8 +5069,11 @@
       <c r="G143" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I143" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="144" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B144" t="s">
         <v>121</v>
       </c>
@@ -4767,8 +5092,11 @@
       <c r="G144" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I144" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="145" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B145" t="s">
         <v>122</v>
       </c>
@@ -4787,8 +5115,11 @@
       <c r="G145" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I145" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="146" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B146" t="s">
         <v>123</v>
       </c>
@@ -4804,8 +5135,11 @@
       <c r="G146" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I146" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="147" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B147" t="s">
         <v>124</v>
       </c>
@@ -4824,8 +5158,11 @@
       <c r="G147" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I147" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="148" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B148" t="s">
         <v>125</v>
       </c>
@@ -4841,8 +5178,11 @@
       <c r="G148" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I148" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="149" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C149" t="s">
         <v>241</v>
       </c>
@@ -4850,7 +5190,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B150" t="s">
         <v>126</v>
       </c>
@@ -4869,8 +5209,11 @@
       <c r="G150" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I150" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="151" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B151" t="s">
         <v>127</v>
       </c>
@@ -4886,8 +5229,11 @@
       <c r="G151" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I151" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="152" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C152" t="s">
         <v>242</v>
       </c>
@@ -4895,7 +5241,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B153" t="s">
         <v>128</v>
       </c>
@@ -4914,8 +5260,11 @@
       <c r="G153" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I153" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="154" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B154" s="2" t="s">
         <v>129</v>
       </c>
@@ -4931,8 +5280,11 @@
       <c r="G154" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I154" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="155" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B155" t="s">
         <v>130</v>
       </c>
@@ -4948,8 +5300,11 @@
       <c r="G155" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I155" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="156" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B156" t="s">
         <v>131</v>
       </c>
@@ -4965,8 +5320,11 @@
       <c r="G156" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I156" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="157" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B157" t="s">
         <v>132</v>
       </c>
@@ -4982,8 +5340,11 @@
       <c r="G157" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I157" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="158" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B158" t="s">
         <v>133</v>
       </c>
@@ -4999,8 +5360,11 @@
       <c r="G158" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I158" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="159" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C159" t="s">
         <v>244</v>
       </c>
@@ -5008,7 +5372,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B160" t="s">
         <v>134</v>
       </c>
@@ -5027,8 +5391,11 @@
       <c r="G160" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="161" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I160" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="161" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B161" t="s">
         <v>135</v>
       </c>
@@ -5047,8 +5414,11 @@
       <c r="G161" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="162" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I161" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="162" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B162" t="s">
         <v>136</v>
       </c>
@@ -5062,7 +5432,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="163" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B163" t="s">
         <v>137</v>
       </c>
@@ -5081,8 +5451,11 @@
       <c r="G163" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="164" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I163" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="164" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B164" t="s">
         <v>138</v>
       </c>
@@ -5093,7 +5466,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="165" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B165" t="s">
         <v>139</v>
       </c>
@@ -5112,8 +5485,11 @@
       <c r="G165" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="166" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I165" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="166" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B166" t="s">
         <v>140</v>
       </c>
@@ -5132,8 +5508,11 @@
       <c r="G166" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="167" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I166" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="167" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B167" t="s">
         <v>141</v>
       </c>
@@ -5144,7 +5523,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="168" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C168" t="s">
         <v>141</v>
       </c>
@@ -5152,7 +5531,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="169" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B169" t="s">
         <v>142</v>
       </c>
@@ -5171,8 +5550,11 @@
       <c r="G169" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="170" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I169" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="170" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B170" t="s">
         <v>143</v>
       </c>
@@ -5188,8 +5570,11 @@
       <c r="G170" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="171" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I170" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="171" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B171" t="s">
         <v>144</v>
       </c>
@@ -5205,8 +5590,11 @@
       <c r="G171" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="172" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I171" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="172" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B172" t="s">
         <v>145</v>
       </c>
@@ -5225,8 +5613,11 @@
       <c r="G172" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="173" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I172" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="173" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B173" t="s">
         <v>146</v>
       </c>
@@ -5239,8 +5630,11 @@
       <c r="G173" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="174" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I173" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="174" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B174" t="s">
         <v>147</v>
       </c>
@@ -5251,7 +5645,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="175" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C175" t="s">
         <v>247</v>
       </c>
@@ -5259,7 +5653,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="176" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C176" t="s">
         <v>104</v>
       </c>
@@ -5267,7 +5661,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="177" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C177" t="s">
         <v>146</v>
       </c>
@@ -5275,7 +5669,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="178" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C178" t="s">
         <v>248</v>
       </c>
@@ -5283,7 +5677,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="179" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C179" t="s">
         <v>147</v>
       </c>
@@ -5291,7 +5685,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="180" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B180" t="s">
         <v>148</v>
       </c>
@@ -5310,8 +5704,11 @@
       <c r="G180" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="181" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I180" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="181" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B181" t="s">
         <v>149</v>
       </c>
@@ -5330,8 +5727,11 @@
       <c r="G181" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="182" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I181" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="182" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B182" t="s">
         <v>150</v>
       </c>
@@ -5350,8 +5750,11 @@
       <c r="G182" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="183" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I182" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="183" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B183" t="s">
         <v>151</v>
       </c>
@@ -5365,12 +5768,12 @@
         <v>161</v>
       </c>
     </row>
-    <row r="184" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F184" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="185" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B185" t="s">
         <v>152</v>
       </c>
@@ -5386,8 +5789,11 @@
       <c r="F185" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="186" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I185" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="186" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B186" t="s">
         <v>153</v>
       </c>
@@ -5400,8 +5806,11 @@
       <c r="E186" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="187" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I186" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="187" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B187" t="s">
         <v>154</v>
       </c>
@@ -5417,8 +5826,11 @@
       <c r="F187" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="188" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I187" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="188" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B188" t="s">
         <v>155</v>
       </c>
@@ -5434,8 +5846,11 @@
       <c r="F188" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="189" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I188" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="189" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B189" t="s">
         <v>156</v>
       </c>
@@ -5451,13 +5866,16 @@
       <c r="F189" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="190" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I189" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="190" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C190" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="191" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B191" t="s">
         <v>157</v>
       </c>
@@ -5473,8 +5891,11 @@
       <c r="F191" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="192" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I191" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="192" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B192" t="s">
         <v>158</v>
       </c>
@@ -5490,8 +5911,11 @@
       <c r="F192" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="193" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I192" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="193" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B193" t="s">
         <v>159</v>
       </c>
@@ -5499,7 +5923,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="194" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B194" t="s">
         <v>160</v>
       </c>
@@ -5515,13 +5939,16 @@
       <c r="F194" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="195" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I194" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="195" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C195" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="196" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B196" t="s">
         <v>161</v>
       </c>
@@ -5537,8 +5964,11 @@
       <c r="F196" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="197" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I196" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="197" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B197" s="2" t="s">
         <v>162</v>
       </c>
@@ -5557,8 +5987,11 @@
       <c r="G197" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="198" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I197" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="198" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B198" t="s">
         <v>163</v>
       </c>
@@ -5577,8 +6010,11 @@
       <c r="G198" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="199" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I198" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="199" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C199" t="s">
         <v>251</v>
       </c>
@@ -5586,7 +6022,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="200" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B200" s="2" t="s">
         <v>182</v>
       </c>
@@ -5602,8 +6038,11 @@
       <c r="G200" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="201" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I200" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="201" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B201" s="2" t="s">
         <v>183</v>
       </c>
@@ -5619,8 +6058,11 @@
       <c r="G201" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="202" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I201" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="202" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B202" t="s">
         <v>184</v>
       </c>
@@ -5631,7 +6073,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="203" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B203" s="2" t="s">
         <v>185</v>
       </c>
@@ -5647,8 +6089,11 @@
       <c r="G203" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="204" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I203" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="204" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B204" t="s">
         <v>164</v>
       </c>
@@ -5664,8 +6109,11 @@
       <c r="G204" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="205" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I204" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="205" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B205" t="s">
         <v>165</v>
       </c>
@@ -5681,8 +6129,11 @@
       <c r="G205" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="206" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I205" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="206" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B206" t="s">
         <v>166</v>
       </c>
@@ -5698,8 +6149,11 @@
       <c r="G206" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="207" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I206" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="207" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B207" t="s">
         <v>167</v>
       </c>
@@ -5718,8 +6172,11 @@
       <c r="G207" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="208" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I207" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="208" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B208" t="s">
         <v>168</v>
       </c>
@@ -5736,10 +6193,13 @@
         <v>168</v>
       </c>
       <c r="G208" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="209" spans="2:7" x14ac:dyDescent="0.3">
+        <v>676</v>
+      </c>
+      <c r="I208" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="209" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B209" t="s">
         <v>169</v>
       </c>
@@ -5758,8 +6218,11 @@
       <c r="G209" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="210" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I209" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="210" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B210" t="s">
         <v>170</v>
       </c>
@@ -5775,8 +6238,11 @@
       <c r="G210" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="211" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I210" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="211" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B211" t="s">
         <v>171</v>
       </c>
@@ -5792,8 +6258,11 @@
       <c r="G211" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="212" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I211" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="212" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B212" t="s">
         <v>172</v>
       </c>
@@ -5812,8 +6281,11 @@
       <c r="G212" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="213" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I212" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="213" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B213" t="s">
         <v>173</v>
       </c>
@@ -5821,7 +6293,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="214" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B214" t="s">
         <v>174</v>
       </c>
@@ -5840,8 +6312,11 @@
       <c r="G214" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="215" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I214" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="215" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B215" t="s">
         <v>175</v>
       </c>
@@ -5860,8 +6335,11 @@
       <c r="G215" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="216" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I215" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="216" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B216" t="s">
         <v>176</v>
       </c>
@@ -5877,8 +6355,11 @@
       <c r="G216" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="217" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I216" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="217" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B217" t="s">
         <v>177</v>
       </c>
@@ -5894,8 +6375,11 @@
       <c r="G217" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="218" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I217" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="218" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B218" t="s">
         <v>178</v>
       </c>
@@ -5912,10 +6396,13 @@
         <v>178</v>
       </c>
       <c r="G218" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="219" spans="2:7" x14ac:dyDescent="0.3">
+        <v>677</v>
+      </c>
+      <c r="I218" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="219" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C219" t="s">
         <v>256</v>
       </c>
@@ -5923,12 +6410,12 @@
         <v>182</v>
       </c>
     </row>
-    <row r="220" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:9" x14ac:dyDescent="0.3">
       <c r="G220" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="221" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B221" t="s">
         <v>179</v>
       </c>
@@ -5942,10 +6429,13 @@
         <v>179</v>
       </c>
       <c r="G221" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="222" spans="2:7" x14ac:dyDescent="0.3">
+        <v>678</v>
+      </c>
+      <c r="I221" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="222" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B222" t="s">
         <v>180</v>
       </c>
@@ -5964,8 +6454,11 @@
       <c r="G222" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="223" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I222" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="223" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B223" t="s">
         <v>181</v>
       </c>
@@ -5984,8 +6477,11 @@
       <c r="G223" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="224" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I223" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="224" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B224" t="s">
         <v>186</v>
       </c>
@@ -6001,8 +6497,11 @@
       <c r="G224" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="225" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I224" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="225" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B225" t="s">
         <v>187</v>
       </c>
@@ -6018,8 +6517,11 @@
       <c r="G225" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="226" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I225" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="226" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C226" t="s">
         <v>257</v>
       </c>
@@ -6027,7 +6529,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="227" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B227" t="s">
         <v>188</v>
       </c>
@@ -6046,8 +6548,11 @@
       <c r="G227" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="228" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I227" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="228" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B228" t="s">
         <v>189</v>
       </c>
@@ -6066,8 +6571,11 @@
       <c r="G228" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="229" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I228" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="229" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B229" t="s">
         <v>190</v>
       </c>
@@ -6083,8 +6591,11 @@
       <c r="G229" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="230" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I229" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="230" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D230" s="2" t="s">
         <v>277</v>
       </c>
@@ -6097,8 +6608,11 @@
       <c r="G230" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="231" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I230" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="231" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B231" t="s">
         <v>191</v>
       </c>
@@ -6112,10 +6626,13 @@
         <v>191</v>
       </c>
       <c r="G231" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="232" spans="2:7" x14ac:dyDescent="0.3">
+        <v>679</v>
+      </c>
+      <c r="I231" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="232" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B232" t="s">
         <v>192</v>
       </c>
@@ -6131,8 +6648,11 @@
       <c r="G232" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="233" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I232" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="233" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B233" t="s">
         <v>193</v>
       </c>
@@ -6151,8 +6671,11 @@
       <c r="G233" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="234" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I233" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="234" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C234" t="s">
         <v>45</v>
       </c>
@@ -6160,7 +6683,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="235" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B235" t="s">
         <v>194</v>
       </c>
@@ -6176,8 +6699,11 @@
       <c r="G235" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="236" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I235" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="236" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B236" t="s">
         <v>195</v>
       </c>
@@ -6193,8 +6719,11 @@
       <c r="F236" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="237" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I236" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="237" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B237" t="s">
         <v>196</v>
       </c>
@@ -6202,7 +6731,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="238" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="238" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B238" t="s">
         <v>197</v>
       </c>
@@ -6215,8 +6744,11 @@
       <c r="F238" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="239" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I238" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="239" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B239" t="s">
         <v>198</v>
       </c>
@@ -6232,8 +6764,11 @@
       <c r="F239" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="240" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I239" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="240" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B240" t="s">
         <v>199</v>
       </c>
@@ -6249,8 +6784,11 @@
       <c r="F240" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="241" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I240" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="241" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B241" t="s">
         <v>200</v>
       </c>
@@ -6258,7 +6796,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="242" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B242" t="s">
         <v>201</v>
       </c>
@@ -6266,7 +6804,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="243" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="243" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B243" t="s">
         <v>202</v>
       </c>
@@ -6274,7 +6812,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="244" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="244" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B244" t="s">
         <v>203</v>
       </c>
@@ -6290,8 +6828,11 @@
       <c r="F244" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="245" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I244" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="245" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B245" t="s">
         <v>204</v>
       </c>
@@ -6307,8 +6848,11 @@
       <c r="F245" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="246" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I245" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="246" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B246" t="s">
         <v>205</v>
       </c>
@@ -6324,8 +6868,11 @@
       <c r="F246" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="247" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I246" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="247" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B247" t="s">
         <v>206</v>
       </c>
@@ -6341,8 +6888,11 @@
       <c r="F247" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="248" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I247" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="248" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B248" s="2" t="s">
         <v>207</v>
       </c>
@@ -6361,13 +6911,16 @@
       <c r="G248" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="249" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I248" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="249" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C249" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="250" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="250" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B250" t="s">
         <v>208</v>
       </c>
@@ -6386,8 +6939,11 @@
       <c r="G250" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="251" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I250" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="251" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B251" t="s">
         <v>209</v>
       </c>
@@ -6403,8 +6959,11 @@
       <c r="G251" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="252" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I251" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="252" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B252" t="s">
         <v>210</v>
       </c>
@@ -6420,8 +6979,11 @@
       <c r="G252" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="253" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I252" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="253" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B253" t="s">
         <v>211</v>
       </c>
@@ -6434,8 +6996,11 @@
       <c r="E253" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="254" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I253" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="254" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B254" t="s">
         <v>212</v>
       </c>
@@ -6454,8 +7019,11 @@
       <c r="G254" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="255" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I254" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="255" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B255" t="s">
         <v>213</v>
       </c>
@@ -6471,8 +7039,11 @@
       <c r="G255" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="256" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I255" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="256" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B256" t="s">
         <v>214</v>
       </c>
@@ -6483,7 +7054,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C257" t="s">
         <v>262</v>
       </c>
@@ -6491,7 +7062,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C258" t="s">
         <v>263</v>
       </c>
@@ -6502,7 +7073,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B259" t="s">
         <v>215</v>
       </c>
@@ -6518,8 +7089,11 @@
       <c r="G259" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I259" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B260" t="s">
         <v>216</v>
       </c>
@@ -6538,8 +7112,11 @@
       <c r="G260" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I260" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B261" t="s">
         <v>217</v>
       </c>
@@ -6555,8 +7132,11 @@
       <c r="F261" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="263" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I261" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
         <v>289</v>
       </c>
@@ -6570,7 +7150,7 @@
       </c>
       <c r="D263" s="1">
         <f t="shared" si="0"/>
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E263" s="1">
         <f t="shared" si="0"/>
@@ -6582,7 +7162,11 @@
       </c>
       <c r="G263" s="1">
         <f>COUNTA(G4:G261)</f>
-        <v>222</v>
+        <v>221</v>
+      </c>
+      <c r="I263" s="1">
+        <f t="shared" ref="H263:I263" si="1">COUNTA(I4:I261)</f>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -6599,8 +7183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F233"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8072,7 +8656,7 @@
   <dimension ref="A1:S481"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>